<commit_message>
use cases refined by waseem. 50% task completed Rest to be done by other member.
</commit_message>
<xml_diff>
--- a/DOCS/Test Cases/TC18-Search Volunteers.xlsx
+++ b/DOCS/Test Cases/TC18-Search Volunteers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="9105" yWindow="-15" windowWidth="9120" windowHeight="9180"/>
   </bookViews>
   <sheets>
     <sheet name="Options" sheetId="1" r:id="rId1"/>
@@ -154,7 +154,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,13 +166,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -308,6 +301,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -322,10 +319,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -624,7 +617,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C10" sqref="C10:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -634,7 +627,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -689,7 +682,7 @@
       <c r="A3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C3" s="6" t="s">
@@ -715,7 +708,7 @@
       <c r="B4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="8" t="s">
         <v>29</v>
       </c>
       <c r="D4" s="6"/>
@@ -885,7 +878,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -903,35 +896,35 @@
       <c r="A1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="9" t="s">
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="11" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
       <c r="C3" s="4" t="s">
         <v>16</v>
       </c>
@@ -943,7 +936,7 @@
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
-      <c r="H3" s="10"/>
+      <c r="H3" s="12"/>
     </row>
     <row r="4" spans="1:8" ht="24.75" customHeight="1" thickTop="1">
       <c r="A4" t="s">

</xml_diff>